<commit_message>
Use PHS XLSX as source for historical deaths. Note that this has shifted the reporting date by one day.
</commit_message>
<xml_diff>
--- a/data/raw/phs/HSCA+-+SG+Website+-+Indicator+Trends+for+daily+data+publication.xlsx
+++ b/data/raw/phs/HSCA+-+SG+Website+-+Indicator+Trends+for+daily+data+publication.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u201433\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA1432\A27932939\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U442507\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA14172\A27932939\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18735" windowHeight="6165" tabRatio="948"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18735" windowHeight="6165" tabRatio="948" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="17" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="94">
   <si>
     <t>Date</t>
   </si>
@@ -468,9 +468,6 @@
   </si>
   <si>
     <t>https://www.nrscotland.gov.uk/covid19stats</t>
-  </si>
-  <si>
-    <t>G drive</t>
   </si>
 </sst>
 </file>
@@ -1355,10 +1352,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Table 1 - NHS 24'!$A$4:$A$40</c:f>
+              <c:f>'Table 1 - NHS 24'!$A$4:$A$41</c:f>
               <c:numCache>
                 <c:formatCode>dd/mm/yy;@</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>43907</c:v>
                 </c:pt>
@@ -1469,16 +1466,19 @@
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>43943</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>43944</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Table 1 - NHS 24'!$B$4:$B$40</c:f>
+              <c:f>'Table 1 - NHS 24'!$B$4:$B$41</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>6977</c:v>
                 </c:pt>
@@ -1589,6 +1589,9 @@
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>3061</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3009</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1649,10 +1652,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Table 1 - NHS 24'!$A$4:$A$40</c:f>
+              <c:f>'Table 1 - NHS 24'!$A$4:$A$41</c:f>
               <c:numCache>
                 <c:formatCode>dd/mm/yy;@</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>43907</c:v>
                 </c:pt>
@@ -1763,16 +1766,19 @@
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>43943</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>43944</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Table 1 - NHS 24'!$C$4:$C$40</c:f>
+              <c:f>'Table 1 - NHS 24'!$C$4:$C$41</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>6772</c:v>
                 </c:pt>
@@ -1883,6 +1889,9 @@
                 </c:pt>
                 <c:pt idx="36" formatCode="General">
                   <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="General">
+                  <c:v>364</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2154,7 +2163,7 @@
               <c:f>'Chart 2 - Hospital Care '!DateHosp</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>43908</c:v>
                 </c:pt>
@@ -2265,6 +2274,9 @@
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>43944</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>43945</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2274,7 +2286,7 @@
               <c:f>'Chart 2 - Hospital Care '!ConfirmedHosp</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>#N/A</c:v>
                 </c:pt>
@@ -2385,6 +2397,9 @@
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>1423</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1383</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2424,7 +2439,7 @@
               <c:f>'Chart 2 - Hospital Care '!DateHosp</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>43908</c:v>
                 </c:pt>
@@ -2535,6 +2550,9 @@
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>43944</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>43945</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2544,7 +2562,7 @@
               <c:f>'Chart 2 - Hospital Care '!SuspectedHosp</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>#N/A</c:v>
                 </c:pt>
@@ -2655,6 +2673,9 @@
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>325</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>327</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2688,7 +2709,7 @@
               <c:f>'Chart 2 - Hospital Care '!DateHosp</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>43908</c:v>
                 </c:pt>
@@ -2799,6 +2820,9 @@
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>43944</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>43945</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2808,7 +2832,7 @@
               <c:f>'Chart 2 - Hospital Care '!UnknownHosp</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>149</c:v>
                 </c:pt>
@@ -2918,6 +2942,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="36">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="37">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3255,7 +3282,7 @@
               <c:f>'Chart 3 - Hospital Care (ICU)'!Date</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>43908</c:v>
                 </c:pt>
@@ -3366,6 +3393,9 @@
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>43944</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>43945</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3375,7 +3405,7 @@
               <c:f>'Chart 3 - Hospital Care (ICU)'!Confirmed</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>#N/A</c:v>
                 </c:pt>
@@ -3485,6 +3515,9 @@
                   <c:v>147</c:v>
                 </c:pt>
                 <c:pt idx="36">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="37">
                   <c:v>136</c:v>
                 </c:pt>
               </c:numCache>
@@ -3525,7 +3558,7 @@
               <c:f>'Chart 3 - Hospital Care (ICU)'!Date</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>43908</c:v>
                 </c:pt>
@@ -3636,6 +3669,9 @@
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>43944</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>43945</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3645,7 +3681,7 @@
               <c:f>'Chart 3 - Hospital Care (ICU)'!Suspected</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>#N/A</c:v>
                 </c:pt>
@@ -3756,6 +3792,9 @@
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3797,7 +3836,7 @@
               <c:f>'Chart 3 - Hospital Care (ICU)'!Date</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>43908</c:v>
                 </c:pt>
@@ -3908,6 +3947,9 @@
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>43944</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>43945</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3917,7 +3959,7 @@
               <c:f>'Chart 3 - Hospital Care (ICU)'!Unknown</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>6</c:v>
                 </c:pt>
@@ -4027,6 +4069,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="36">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="37">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -4445,10 +4490,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Table 3 - Ambulance'!$A$4:$A$39</c:f>
+              <c:f>'Table 3 - Ambulance'!$A$4:$A$40</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>43908</c:v>
                 </c:pt>
@@ -4556,16 +4601,19 @@
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>43943</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>43944</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Table 3 - Ambulance'!$B$4:$B$39</c:f>
+              <c:f>'Table 3 - Ambulance'!$B$4:$B$40</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>1525</c:v>
                 </c:pt>
@@ -4673,6 +4721,9 @@
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>1389</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1489</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4733,10 +4784,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Table 3 - Ambulance'!$A$4:$A$39</c:f>
+              <c:f>'Table 3 - Ambulance'!$A$4:$A$40</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>43908</c:v>
                 </c:pt>
@@ -4844,16 +4895,19 @@
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>43943</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>43944</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Table 3 - Ambulance'!$C$4:$C$39</c:f>
+              <c:f>'Table 3 - Ambulance'!$C$4:$C$40</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>286</c:v>
                 </c:pt>
@@ -4961,6 +5015,9 @@
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>307</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>327</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4992,7 +5049,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="dd/mm/yy;@" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5297,10 +5354,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Table 3 - Ambulance'!$A$4:$A$39</c:f>
+              <c:f>'Table 3 - Ambulance'!$A$4:$A$40</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>43908</c:v>
                 </c:pt>
@@ -5408,16 +5465,19 @@
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>43943</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>43944</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Table 3 - Ambulance'!$D$4:$D$39</c:f>
+              <c:f>'Table 3 - Ambulance'!$D$4:$D$40</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>176</c:v>
                 </c:pt>
@@ -5525,6 +5585,9 @@
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>205</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5556,7 +5619,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="dd/mm/yy;@" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5781,7 +5844,7 @@
           <c:yMode val="edge"/>
           <c:x val="6.6168795199050209E-2"/>
           <c:y val="0.11653757239535749"/>
-          <c:w val="0.86661328729480458"/>
+          <c:w val="0.89830950732263137"/>
           <c:h val="0.69065621356861318"/>
         </c:manualLayout>
       </c:layout>
@@ -5805,8 +5868,13 @@
           </c:marker>
           <c:dLbls>
             <c:dLbl>
-              <c:idx val="33"/>
-              <c:layout/>
+              <c:idx val="34"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.6941762989604771E-2"/>
+                  <c:y val="-5.4807987552113442E-3"/>
+                </c:manualLayout>
+              </c:layout>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -5814,11 +5882,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000000-AA21-48E5-9BB4-25AAF597C014}"/>
+                  <c16:uniqueId val="{00000000-585B-4278-940F-442115C9565D}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -5836,7 +5902,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -5859,30 +5925,16 @@
             <c:showBubbleSize val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
+                <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'Table 4 - Delayed Discharge'!$A$4:$A$37</c:f>
+              <c:f>'Table 4 - Delayed Discharge'!$A$4:$A$38</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>43894</c:v>
                 </c:pt>
@@ -5984,21 +6036,24 @@
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>43943</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>43944</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Table 4 - Delayed Discharge'!$B$4:$B$37</c:f>
+              <c:f>'Table 4 - Delayed Discharge'!$B$4:$B$38</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>1612</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1563</c:v>
+                  <c:v>1533</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1553</c:v>
@@ -6034,13 +6089,13 @@
                   <c:v>1200</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1166</c:v>
+                  <c:v>1120</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1130</c:v>
+                  <c:v>1090</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1115</c:v>
+                  <c:v>1075</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>1041</c:v>
@@ -6095,6 +6150,9 @@
                 </c:pt>
                 <c:pt idx="33" formatCode="General">
                   <c:v>610</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="General">
+                  <c:v>600</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6125,7 +6183,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="dd/mm/yy;@" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -6143,7 +6201,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -6311,7 +6369,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6366,10 +6423,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Table 5 - Testing'!$A$5:$A$57</c:f>
+              <c:f>'Table 5 - Testing'!$A$5:$A$58</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="53"/>
+                <c:ptCount val="54"/>
                 <c:pt idx="0">
                   <c:v>43892</c:v>
                 </c:pt>
@@ -6528,16 +6585,19 @@
                 </c:pt>
                 <c:pt idx="52">
                   <c:v>43944</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>43945</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Table 5 - Testing'!$C$5:$C$57</c:f>
+              <c:f>'Table 5 - Testing'!$C$5:$C$58</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="53"/>
+                <c:ptCount val="54"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -6696,6 +6756,9 @@
                 </c:pt>
                 <c:pt idx="52">
                   <c:v>9409</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>9697</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6724,10 +6787,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Table 5 - Testing'!$A$5:$A$57</c:f>
+              <c:f>'Table 5 - Testing'!$A$5:$A$58</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="53"/>
+                <c:ptCount val="54"/>
                 <c:pt idx="0">
                   <c:v>43892</c:v>
                 </c:pt>
@@ -6886,16 +6949,19 @@
                 </c:pt>
                 <c:pt idx="52">
                   <c:v>43944</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>43945</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Table 5 - Testing'!$B$5:$B$57</c:f>
+              <c:f>'Table 5 - Testing'!$B$5:$B$58</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="53"/>
+                <c:ptCount val="54"/>
                 <c:pt idx="0">
                   <c:v>814</c:v>
                 </c:pt>
@@ -7054,6 +7120,9 @@
                 </c:pt>
                 <c:pt idx="52">
                   <c:v>35390</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>36392</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7381,10 +7450,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Table 6 - Workforce'!$A$18:$A$39</c:f>
+              <c:f>'Table 6 - Workforce'!$A$18:$A$40</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>43922</c:v>
                 </c:pt>
@@ -7450,16 +7519,19 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>43943</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43944</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Table 6 - Workforce'!$B$18:$B$39</c:f>
+              <c:f>'Table 6 - Workforce'!$B$18:$B$40</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>4354</c:v>
                 </c:pt>
@@ -7525,6 +7597,9 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>3434</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3496</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7564,10 +7639,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Table 6 - Workforce'!$A$18:$A$39</c:f>
+              <c:f>'Table 6 - Workforce'!$A$18:$A$40</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>43922</c:v>
                 </c:pt>
@@ -7633,16 +7708,19 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>43943</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43944</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Table 6 - Workforce'!$C$18:$C$39</c:f>
+              <c:f>'Table 6 - Workforce'!$C$18:$C$40</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>467</c:v>
                 </c:pt>
@@ -7708,6 +7786,9 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>233</c:v>
+                </c:pt>
+                <c:pt idx="22" formatCode="General">
+                  <c:v>237</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7746,10 +7827,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Table 6 - Workforce'!$A$18:$A$39</c:f>
+              <c:f>'Table 6 - Workforce'!$A$18:$A$40</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>43922</c:v>
                 </c:pt>
@@ -7815,16 +7896,19 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>43943</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43944</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Table 6 - Workforce'!$D$18:$D$39</c:f>
+              <c:f>'Table 6 - Workforce'!$D$18:$D$40</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>4898</c:v>
                 </c:pt>
@@ -7890,6 +7974,9 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>3680</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3834</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8115,7 +8202,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15427,15 +15513,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>757806</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>128798</xdr:rowOff>
+      <xdr:colOff>729052</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>109628</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>383596</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>169333</xdr:rowOff>
+      <xdr:colOff>354842</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>150163</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -15444,8 +15530,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4059806" y="3938798"/>
-          <a:ext cx="4144873" cy="2136035"/>
+          <a:off x="4131693" y="1048949"/>
+          <a:ext cx="4255300" cy="2043780"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16879,8 +16965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16891,13 +16977,13 @@
     <col min="4" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="23.85" x14ac:dyDescent="0.4">
       <c r="A1" s="54" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
         <v>23</v>
       </c>
@@ -17105,7 +17191,7 @@
     <col min="1" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A1" s="46"/>
       <c r="P1" s="33" t="s">
         <v>35</v>
@@ -17129,10 +17215,10 @@
   <dimension ref="A1:N76"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B36" sqref="B36"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17142,7 +17228,7 @@
     <col min="3" max="3" width="3.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>41</v>
       </c>
@@ -17151,11 +17237,11 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:14" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="27.2" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>0</v>
       </c>
@@ -17164,7 +17250,7 @@
       </c>
       <c r="C3" s="67"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A4" s="18">
         <v>43894</v>
       </c>
@@ -17173,16 +17259,16 @@
       </c>
       <c r="C4" s="75"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A5" s="19">
         <v>43899</v>
       </c>
       <c r="B5" s="71">
-        <v>1563</v>
+        <v>1533</v>
       </c>
       <c r="C5" s="75"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A6" s="19">
         <v>43900</v>
       </c>
@@ -17191,7 +17277,7 @@
       </c>
       <c r="C6" s="75"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A7" s="19">
         <v>43901</v>
       </c>
@@ -17200,7 +17286,7 @@
       </c>
       <c r="C7" s="75"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A8" s="19">
         <v>43902</v>
       </c>
@@ -17209,7 +17295,7 @@
       </c>
       <c r="C8" s="75"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A9" s="19">
         <v>43903</v>
       </c>
@@ -17219,7 +17305,7 @@
       <c r="C9" s="75"/>
       <c r="E9" s="44"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A10" s="19">
         <v>43906</v>
       </c>
@@ -17227,8 +17313,9 @@
         <v>1492</v>
       </c>
       <c r="C10" s="75"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D10" s="11"/>
+    </row>
+    <row r="11" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A11" s="19">
         <v>43907</v>
       </c>
@@ -17236,8 +17323,9 @@
         <v>1487</v>
       </c>
       <c r="C11" s="75"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D11" s="11"/>
+    </row>
+    <row r="12" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A12" s="19">
         <v>43908</v>
       </c>
@@ -17257,7 +17345,7 @@
       <c r="M12" s="12"/>
       <c r="N12" s="12"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A13" s="19">
         <v>43909</v>
       </c>
@@ -17277,7 +17365,7 @@
       <c r="M13" s="12"/>
       <c r="N13" s="12"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A14" s="19">
         <v>43910</v>
       </c>
@@ -17297,7 +17385,7 @@
       <c r="M14" s="12"/>
       <c r="N14" s="12"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A15" s="19">
         <v>43913</v>
       </c>
@@ -17317,7 +17405,7 @@
       <c r="M15" s="12"/>
       <c r="N15" s="12"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A16" s="19">
         <v>43914</v>
       </c>
@@ -17337,12 +17425,12 @@
       <c r="M16" s="12"/>
       <c r="N16" s="12"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A17" s="19">
         <v>43915</v>
       </c>
       <c r="B17" s="71">
-        <v>1166</v>
+        <v>1120</v>
       </c>
       <c r="C17" s="75"/>
       <c r="D17" s="11"/>
@@ -17357,12 +17445,12 @@
       <c r="M17" s="12"/>
       <c r="N17" s="12"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A18" s="19">
         <v>43916</v>
       </c>
       <c r="B18" s="71">
-        <v>1130</v>
+        <v>1090</v>
       </c>
       <c r="C18" s="75"/>
       <c r="D18" s="11"/>
@@ -17377,12 +17465,12 @@
       <c r="M18" s="12"/>
       <c r="N18" s="12"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A19" s="19">
         <v>43917</v>
       </c>
       <c r="B19" s="71">
-        <v>1115</v>
+        <v>1075</v>
       </c>
       <c r="C19" s="75"/>
       <c r="D19" s="11"/>
@@ -17397,7 +17485,7 @@
       <c r="M19" s="12"/>
       <c r="N19" s="12"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A20" s="19">
         <v>43920</v>
       </c>
@@ -17417,7 +17505,7 @@
       <c r="M20" s="12"/>
       <c r="N20" s="12"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A21" s="19">
         <v>43921</v>
       </c>
@@ -17437,7 +17525,7 @@
       <c r="M21" s="12"/>
       <c r="N21" s="12"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A22" s="19">
         <v>43922</v>
       </c>
@@ -17457,7 +17545,7 @@
       <c r="M22" s="12"/>
       <c r="N22" s="12"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A23" s="19">
         <v>43923</v>
       </c>
@@ -17477,7 +17565,7 @@
       <c r="M23" s="12"/>
       <c r="N23" s="12"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A24" s="19">
         <v>43924</v>
       </c>
@@ -17485,7 +17573,6 @@
         <v>805</v>
       </c>
       <c r="C24" s="75"/>
-      <c r="D24" s="11"/>
       <c r="E24" s="11"/>
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
@@ -17497,7 +17584,7 @@
       <c r="M24" s="12"/>
       <c r="N24" s="12"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A25" s="19">
         <v>43927</v>
       </c>
@@ -17505,7 +17592,6 @@
         <v>740</v>
       </c>
       <c r="C25" s="75"/>
-      <c r="D25" s="11"/>
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
       <c r="G25" s="11"/>
@@ -17517,7 +17603,7 @@
       <c r="M25" s="12"/>
       <c r="N25" s="12"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A26" s="19">
         <v>43928</v>
       </c>
@@ -17525,7 +17611,6 @@
         <v>725</v>
       </c>
       <c r="C26" s="75"/>
-      <c r="D26" s="11"/>
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
       <c r="G26" s="11"/>
@@ -17537,7 +17622,7 @@
       <c r="M26" s="12"/>
       <c r="N26" s="12"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A27" s="19">
         <v>43929</v>
       </c>
@@ -17545,7 +17630,6 @@
         <v>692</v>
       </c>
       <c r="C27" s="75"/>
-      <c r="D27" s="11"/>
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
       <c r="G27" s="11"/>
@@ -17565,7 +17649,6 @@
         <v>687</v>
       </c>
       <c r="C28" s="75"/>
-      <c r="D28" s="11"/>
       <c r="E28" s="11"/>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
@@ -17585,7 +17668,6 @@
         <v>652</v>
       </c>
       <c r="C29" s="75"/>
-      <c r="D29" s="11"/>
       <c r="E29" s="11"/>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
@@ -17670,6 +17752,12 @@
       <c r="C37" s="45"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="21">
+        <v>43944</v>
+      </c>
+      <c r="B38" s="2">
+        <v>600</v>
+      </c>
       <c r="C38" s="45"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -17803,16 +17891,14 @@
   </sheetPr>
   <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
       <c r="P1" s="33" t="s">
         <v>35</v>
@@ -17837,13 +17923,13 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:P57"/>
+  <dimension ref="A1:P58"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="G59" sqref="G59"/>
+      <selection pane="bottomRight" activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17853,7 +17939,7 @@
     <col min="5" max="5" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
@@ -17864,7 +17950,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -17894,7 +17980,7 @@
       </c>
       <c r="E4" s="76"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A5" s="39">
         <v>43892</v>
       </c>
@@ -17920,7 +18006,7 @@
       <c r="O5" s="12"/>
       <c r="P5" s="12"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A6" s="39">
         <v>43893</v>
       </c>
@@ -17946,7 +18032,7 @@
       <c r="O6" s="12"/>
       <c r="P6" s="12"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A7" s="39">
         <v>43894</v>
       </c>
@@ -17972,7 +18058,7 @@
       <c r="O7" s="12"/>
       <c r="P7" s="12"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A8" s="39">
         <v>43895</v>
       </c>
@@ -17998,7 +18084,7 @@
       <c r="O8" s="12"/>
       <c r="P8" s="12"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A9" s="39">
         <v>43896</v>
       </c>
@@ -18024,7 +18110,7 @@
       <c r="O9" s="12"/>
       <c r="P9" s="12"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A10" s="39">
         <v>43897</v>
       </c>
@@ -18050,7 +18136,7 @@
       <c r="O10" s="12"/>
       <c r="P10" s="12"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A11" s="39">
         <v>43898</v>
       </c>
@@ -18076,7 +18162,7 @@
       <c r="O11" s="12"/>
       <c r="P11" s="12"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A12" s="39">
         <v>43899</v>
       </c>
@@ -18102,7 +18188,7 @@
       <c r="O12" s="12"/>
       <c r="P12" s="12"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A13" s="39">
         <v>43900</v>
       </c>
@@ -18128,7 +18214,7 @@
       <c r="O13" s="12"/>
       <c r="P13" s="12"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A14" s="39">
         <v>43901</v>
       </c>
@@ -18154,7 +18240,7 @@
       <c r="O14" s="12"/>
       <c r="P14" s="12"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A15" s="39">
         <v>43902</v>
       </c>
@@ -18180,7 +18266,7 @@
       <c r="O15" s="12"/>
       <c r="P15" s="12"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A16" s="39">
         <v>43903</v>
       </c>
@@ -18206,7 +18292,7 @@
       <c r="O16" s="12"/>
       <c r="P16" s="12"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A17" s="39">
         <v>43904</v>
       </c>
@@ -18232,7 +18318,7 @@
       <c r="O17" s="12"/>
       <c r="P17" s="12"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A18" s="39">
         <v>43905</v>
       </c>
@@ -18258,7 +18344,7 @@
       <c r="O18" s="12"/>
       <c r="P18" s="12"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A19" s="39">
         <v>43906</v>
       </c>
@@ -18284,7 +18370,7 @@
       <c r="O19" s="12"/>
       <c r="P19" s="12"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A20" s="39">
         <v>43907</v>
       </c>
@@ -18310,7 +18396,7 @@
       <c r="O20" s="12"/>
       <c r="P20" s="12"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A21" s="39">
         <v>43908</v>
       </c>
@@ -18336,7 +18422,7 @@
       <c r="O21" s="12"/>
       <c r="P21" s="12"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A22" s="39">
         <v>43909</v>
       </c>
@@ -18362,7 +18448,7 @@
       <c r="O22" s="12"/>
       <c r="P22" s="12"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A23" s="39">
         <v>43910</v>
       </c>
@@ -18388,7 +18474,7 @@
       <c r="O23" s="12"/>
       <c r="P23" s="12"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A24" s="39">
         <v>43911</v>
       </c>
@@ -18414,7 +18500,7 @@
       <c r="O24" s="12"/>
       <c r="P24" s="12"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A25" s="39">
         <v>43912</v>
       </c>
@@ -18440,7 +18526,7 @@
       <c r="O25" s="12"/>
       <c r="P25" s="12"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A26" s="39">
         <v>43913</v>
       </c>
@@ -18466,7 +18552,7 @@
       <c r="O26" s="12"/>
       <c r="P26" s="12"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A27" s="39">
         <v>43914</v>
       </c>
@@ -18492,7 +18578,7 @@
       <c r="O27" s="12"/>
       <c r="P27" s="12"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A28" s="39">
         <v>43915</v>
       </c>
@@ -18518,7 +18604,7 @@
       <c r="O28" s="12"/>
       <c r="P28" s="12"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A29" s="39">
         <v>43916</v>
       </c>
@@ -18544,7 +18630,7 @@
       <c r="O29" s="12"/>
       <c r="P29" s="12"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A30" s="39">
         <v>43917</v>
       </c>
@@ -18559,7 +18645,7 @@
       </c>
       <c r="E30" s="45"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A31" s="39">
         <v>43918</v>
       </c>
@@ -18574,7 +18660,7 @@
       </c>
       <c r="E31" s="45"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A32" s="39">
         <v>43919</v>
       </c>
@@ -18589,7 +18675,7 @@
       </c>
       <c r="E32" s="45"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A33" s="39">
         <v>43920</v>
       </c>
@@ -18604,7 +18690,7 @@
       </c>
       <c r="E33" s="45"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A34" s="39">
         <v>43921</v>
       </c>
@@ -18619,7 +18705,7 @@
       </c>
       <c r="E34" s="45"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A35" s="39">
         <v>43922</v>
       </c>
@@ -18634,7 +18720,7 @@
       </c>
       <c r="E35" s="45"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A36" s="39">
         <v>43923</v>
       </c>
@@ -18649,7 +18735,7 @@
       </c>
       <c r="E36" s="45"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A37" s="39">
         <v>43924</v>
       </c>
@@ -18664,7 +18750,7 @@
       </c>
       <c r="E37" s="45"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A38" s="39">
         <v>43925</v>
       </c>
@@ -18679,7 +18765,7 @@
       </c>
       <c r="E38" s="45"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A39" s="39">
         <v>43926</v>
       </c>
@@ -18694,7 +18780,7 @@
       </c>
       <c r="E39" s="45"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A40" s="39">
         <v>43927</v>
       </c>
@@ -18709,7 +18795,7 @@
       </c>
       <c r="E40" s="45"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A41" s="39">
         <v>43928</v>
       </c>
@@ -18724,7 +18810,7 @@
       </c>
       <c r="E41" s="45"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A42" s="39">
         <v>43929</v>
       </c>
@@ -18739,7 +18825,7 @@
       </c>
       <c r="E42" s="45"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A43" s="39">
         <v>43930</v>
       </c>
@@ -18754,7 +18840,7 @@
       </c>
       <c r="E43" s="45"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A44" s="39">
         <v>43931</v>
       </c>
@@ -18769,7 +18855,7 @@
       </c>
       <c r="E44" s="45"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A45" s="39">
         <v>43932</v>
       </c>
@@ -18784,7 +18870,7 @@
       </c>
       <c r="E45" s="45"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A46" s="39">
         <v>43933</v>
       </c>
@@ -18799,7 +18885,7 @@
       </c>
       <c r="E46" s="45"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A47" s="39">
         <v>43934</v>
       </c>
@@ -18814,7 +18900,7 @@
       </c>
       <c r="E47" s="45"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A48" s="57">
         <v>43935</v>
       </c>
@@ -18829,7 +18915,7 @@
       </c>
       <c r="E48" s="45"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A49" s="21">
         <v>43936</v>
       </c>
@@ -18844,7 +18930,7 @@
       </c>
       <c r="E49" s="45"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A50" s="21">
         <v>43937</v>
       </c>
@@ -18859,7 +18945,7 @@
       </c>
       <c r="E50" s="45"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A51" s="21">
         <v>43938</v>
       </c>
@@ -18873,7 +18959,7 @@
         <v>36637</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A52" s="21">
         <v>43939</v>
       </c>
@@ -18887,7 +18973,7 @@
         <v>38233</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A53" s="21">
         <v>43940</v>
       </c>
@@ -18901,7 +18987,7 @@
         <v>39612</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A54" s="21">
         <v>43941</v>
       </c>
@@ -18915,7 +19001,7 @@
         <v>40700</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A55" s="21">
         <v>43942</v>
       </c>
@@ -18930,7 +19016,7 @@
       </c>
       <c r="E55" s="45"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A56" s="21">
         <v>43943</v>
       </c>
@@ -18945,7 +19031,7 @@
       </c>
       <c r="E56" s="45"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A57" s="21">
         <v>43944</v>
       </c>
@@ -18959,6 +19045,20 @@
         <v>44799</v>
       </c>
       <c r="E57" s="45"/>
+    </row>
+    <row r="58" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A58" s="21">
+        <v>43945</v>
+      </c>
+      <c r="B58" s="100">
+        <v>36392</v>
+      </c>
+      <c r="C58" s="100">
+        <v>9697</v>
+      </c>
+      <c r="D58" s="17">
+        <v>46089</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -18979,10 +19079,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:R20"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18990,13 +19090,8 @@
     <col min="1" max="16384" width="8.85546875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A1" s="43"/>
-    </row>
-    <row r="20" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R20" s="7" t="s">
-        <v>94</v>
-      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -19015,10 +19110,10 @@
   <dimension ref="A1:P44"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E42" sqref="E42"/>
+      <selection pane="bottomRight" activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19027,7 +19122,7 @@
     <col min="2" max="5" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>42</v>
       </c>
@@ -19038,7 +19133,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -19061,7 +19156,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A4" s="18">
         <v>43908</v>
       </c>
@@ -19081,7 +19176,7 @@
       <c r="O4" s="12"/>
       <c r="P4" s="12"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A5" s="19">
         <v>43909</v>
       </c>
@@ -19101,7 +19196,7 @@
       <c r="O5" s="12"/>
       <c r="P5" s="12"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A6" s="19">
         <v>43910</v>
       </c>
@@ -19121,7 +19216,7 @@
       <c r="O6" s="12"/>
       <c r="P6" s="12"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A7" s="19">
         <v>43911</v>
       </c>
@@ -19141,7 +19236,7 @@
       <c r="O7" s="12"/>
       <c r="P7" s="12"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A8" s="19">
         <v>43912</v>
       </c>
@@ -19161,7 +19256,7 @@
       <c r="O8" s="12"/>
       <c r="P8" s="12"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A9" s="19">
         <v>43913</v>
       </c>
@@ -19181,7 +19276,7 @@
       <c r="O9" s="12"/>
       <c r="P9" s="12"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A10" s="19">
         <v>43914</v>
       </c>
@@ -19201,7 +19296,7 @@
       <c r="O10" s="12"/>
       <c r="P10" s="12"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A11" s="19">
         <v>43915</v>
       </c>
@@ -19221,7 +19316,7 @@
       <c r="O11" s="12"/>
       <c r="P11" s="12"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A12" s="19">
         <v>43916</v>
       </c>
@@ -19241,7 +19336,7 @@
       <c r="O12" s="12"/>
       <c r="P12" s="12"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A13" s="19">
         <v>43917</v>
       </c>
@@ -19261,7 +19356,7 @@
       <c r="O13" s="12"/>
       <c r="P13" s="12"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A14" s="19">
         <v>43918</v>
       </c>
@@ -19281,7 +19376,7 @@
       <c r="O14" s="12"/>
       <c r="P14" s="12"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A15" s="19">
         <v>43919</v>
       </c>
@@ -19301,7 +19396,7 @@
       <c r="O15" s="12"/>
       <c r="P15" s="12"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A16" s="19">
         <v>43920</v>
       </c>
@@ -19321,7 +19416,7 @@
       <c r="O16" s="12"/>
       <c r="P16" s="12"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A17" s="19">
         <v>43921</v>
       </c>
@@ -19341,7 +19436,7 @@
       <c r="O17" s="12"/>
       <c r="P17" s="12"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A18" s="19">
         <v>43922</v>
       </c>
@@ -19370,7 +19465,7 @@
       <c r="O18" s="12"/>
       <c r="P18" s="12"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A19" s="19">
         <v>43923</v>
       </c>
@@ -19399,7 +19494,7 @@
       <c r="O19" s="12"/>
       <c r="P19" s="12"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A20" s="19">
         <v>43924</v>
       </c>
@@ -19428,7 +19523,7 @@
       <c r="O20" s="12"/>
       <c r="P20" s="12"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A21" s="19">
         <v>43925</v>
       </c>
@@ -19457,7 +19552,7 @@
       <c r="O21" s="12"/>
       <c r="P21" s="12"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A22" s="19">
         <v>43926</v>
       </c>
@@ -19486,7 +19581,7 @@
       <c r="O22" s="12"/>
       <c r="P22" s="12"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A23" s="19">
         <v>43927</v>
       </c>
@@ -19515,7 +19610,7 @@
       <c r="O23" s="12"/>
       <c r="P23" s="12"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A24" s="19">
         <v>43928</v>
       </c>
@@ -19544,7 +19639,7 @@
       <c r="O24" s="12"/>
       <c r="P24" s="12"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A25" s="19">
         <v>43929</v>
       </c>
@@ -19573,7 +19668,7 @@
       <c r="O25" s="12"/>
       <c r="P25" s="12"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A26" s="19">
         <v>43930</v>
       </c>
@@ -19602,7 +19697,7 @@
       <c r="O26" s="12"/>
       <c r="P26" s="12"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A27" s="19">
         <v>43931</v>
       </c>
@@ -19631,7 +19726,7 @@
       <c r="O27" s="12"/>
       <c r="P27" s="12"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A28" s="21">
         <v>43932</v>
       </c>
@@ -19660,7 +19755,7 @@
       <c r="O28" s="12"/>
       <c r="P28" s="12"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A29" s="21">
         <v>43933</v>
       </c>
@@ -19679,7 +19774,7 @@
       </c>
       <c r="H29" s="12"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A30" s="21">
         <v>43934</v>
       </c>
@@ -19698,7 +19793,7 @@
       </c>
       <c r="H30" s="12"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A31" s="21">
         <v>43935</v>
       </c>
@@ -19716,7 +19811,7 @@
         <v>7093</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A32" s="21">
         <v>43936</v>
       </c>
@@ -19734,7 +19829,7 @@
         <v>7335</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A33" s="21">
         <v>43937</v>
       </c>
@@ -19752,7 +19847,7 @@
         <v>7652</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A34" s="21">
         <v>43938</v>
       </c>
@@ -19770,7 +19865,7 @@
         <v>7931</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A35" s="21">
         <v>43939</v>
       </c>
@@ -19788,7 +19883,7 @@
         <v>7342</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A36" s="21">
         <v>43940</v>
       </c>
@@ -19806,7 +19901,7 @@
         <v>7510</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A37" s="21">
         <v>43941</v>
       </c>
@@ -19823,7 +19918,7 @@
         <v>6971</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A38" s="21">
         <v>43942</v>
       </c>
@@ -19840,7 +19935,7 @@
         <v>7210</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A39" s="21">
         <v>43943</v>
       </c>
@@ -19858,14 +19953,24 @@
         <v>7347</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="21"/>
-      <c r="B40" s="9"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="81"/>
-      <c r="E40" s="71"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A40" s="21">
+        <v>43944</v>
+      </c>
+      <c r="B40" s="9">
+        <v>3496</v>
+      </c>
+      <c r="C40" s="2">
+        <v>237</v>
+      </c>
+      <c r="D40" s="81">
+        <v>3834</v>
+      </c>
+      <c r="E40" s="71">
+        <v>7567</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A41" s="21"/>
       <c r="B41" s="9"/>
       <c r="C41" s="2"/>
@@ -19911,7 +20016,7 @@
   <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="V23" sqref="V23"/>
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19919,7 +20024,7 @@
     <col min="1" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
       <c r="Q1" s="33" t="s">
         <v>35</v>
@@ -19942,9 +20047,7 @@
   </sheetPr>
   <dimension ref="A1:U31"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -19959,7 +20062,7 @@
     <col min="10" max="10" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>80</v>
       </c>
@@ -20012,7 +20115,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A4" s="36">
         <v>43932</v>
       </c>
@@ -20048,7 +20151,7 @@
       <c r="Q4" s="12"/>
       <c r="R4" s="12"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A5" s="36">
         <v>43933</v>
       </c>
@@ -20076,7 +20179,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A6" s="36">
         <v>43934</v>
       </c>
@@ -20104,7 +20207,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A7" s="36">
         <v>43935</v>
       </c>
@@ -20132,7 +20235,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A8" s="73">
         <v>43936</v>
       </c>
@@ -20160,7 +20263,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A9" s="73">
         <v>43937</v>
       </c>
@@ -20188,7 +20291,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A10" s="73">
         <v>43938</v>
       </c>
@@ -20216,7 +20319,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A11" s="73">
         <v>43939</v>
       </c>
@@ -20244,7 +20347,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A12" s="73">
         <v>43940</v>
       </c>
@@ -20272,7 +20375,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A13" s="73">
         <v>43941</v>
       </c>
@@ -20300,7 +20403,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A14" s="73">
         <v>43942</v>
       </c>
@@ -20328,7 +20431,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A15" s="73">
         <v>43943</v>
       </c>
@@ -20356,11 +20459,33 @@
         <v>208</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="C16" s="79"/>
-      <c r="D16" s="79"/>
-      <c r="E16" s="79"/>
-      <c r="F16" s="79"/>
+    <row r="16" spans="1:21" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="73">
+        <v>43944</v>
+      </c>
+      <c r="B16" s="85">
+        <v>516</v>
+      </c>
+      <c r="C16" s="113">
+        <v>0.48</v>
+      </c>
+      <c r="D16" s="133">
+        <v>332</v>
+      </c>
+      <c r="E16" s="131"/>
+      <c r="F16" s="115" t="s">
+        <v>87</v>
+      </c>
+      <c r="G16" s="132" t="s">
+        <v>87</v>
+      </c>
+      <c r="H16" s="130"/>
+      <c r="I16" s="114">
+        <v>2445</v>
+      </c>
+      <c r="J16" s="114">
+        <v>152</v>
+      </c>
     </row>
     <row r="17" spans="1:10" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="149"/>
@@ -20374,13 +20499,13 @@
       <c r="I17" s="149"/>
       <c r="J17" s="149"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="14.25" x14ac:dyDescent="0.25">
       <c r="C18" s="79"/>
       <c r="D18" s="79"/>
       <c r="E18" s="79"/>
       <c r="F18" s="79"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="14.25" x14ac:dyDescent="0.25">
       <c r="C19" s="79"/>
       <c r="D19" s="79"/>
       <c r="E19" s="79"/>
@@ -20484,19 +20609,19 @@
       <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" style="7" customWidth="1"/>
     <col min="2" max="2" width="26" style="7" customWidth="1"/>
-    <col min="3" max="16384" width="8.7109375" style="7"/>
+    <col min="3" max="16384" width="8.5703125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A1" s="118" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="39" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="40.700000000000003" x14ac:dyDescent="0.25">
       <c r="A3" s="119" t="s">
         <v>0</v>
       </c>
@@ -20504,7 +20629,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A4" s="121">
         <v>43903</v>
       </c>
@@ -20512,7 +20637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A5" s="121">
         <v>43904</v>
       </c>
@@ -20520,7 +20645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A6" s="121">
         <v>43905</v>
       </c>
@@ -20528,7 +20653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A7" s="121">
         <v>43906</v>
       </c>
@@ -20536,7 +20661,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A8" s="121">
         <v>43907</v>
       </c>
@@ -20544,7 +20669,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A9" s="121">
         <v>43908</v>
       </c>
@@ -20552,7 +20677,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A10" s="121">
         <v>43909</v>
       </c>
@@ -20560,7 +20685,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A11" s="121">
         <v>43910</v>
       </c>
@@ -20568,7 +20693,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A12" s="121">
         <v>43911</v>
       </c>
@@ -20576,7 +20701,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A13" s="121">
         <v>43912</v>
       </c>
@@ -20584,7 +20709,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A14" s="121">
         <v>43913</v>
       </c>
@@ -20592,7 +20717,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A15" s="121">
         <v>43914</v>
       </c>
@@ -20600,7 +20725,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A16" s="121">
         <v>43915</v>
       </c>
@@ -20608,7 +20733,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A17" s="121">
         <v>43916</v>
       </c>
@@ -20616,7 +20741,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A18" s="121">
         <v>43917</v>
       </c>
@@ -20624,7 +20749,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A19" s="121">
         <v>43918</v>
       </c>
@@ -20853,9 +20978,9 @@
       <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="8.7109375" style="7"/>
+    <col min="1" max="16384" width="8.5703125" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -20881,29 +21006,29 @@
     <col min="1" max="1" width="4.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" ht="14.25" x14ac:dyDescent="0.25">
       <c r="M5" s="55" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B6" s="33" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" ht="14.25" x14ac:dyDescent="0.25">
       <c r="L10" s="33"/>
     </row>
-    <row r="15" spans="2:13" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:13" ht="21.2" x14ac:dyDescent="0.35">
       <c r="B15" s="56"/>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:13" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B16" s="55"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B17" s="33"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B18" s="33" t="s">
         <v>65</v>
       </c>
@@ -20924,7 +21049,7 @@
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:O40"/>
+  <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
@@ -20941,7 +21066,7 @@
     <col min="4" max="4" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>79</v>
       </c>
@@ -20952,7 +21077,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -20970,7 +21095,7 @@
       </c>
       <c r="D3" s="45"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A4" s="34">
         <v>43907</v>
       </c>
@@ -20993,7 +21118,7 @@
       <c r="N4" s="12"/>
       <c r="O4" s="12"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A5" s="35">
         <v>43908</v>
       </c>
@@ -21016,7 +21141,7 @@
       <c r="N5" s="12"/>
       <c r="O5" s="12"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A6" s="35">
         <v>43909</v>
       </c>
@@ -21039,7 +21164,7 @@
       <c r="N6" s="12"/>
       <c r="O6" s="12"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A7" s="35">
         <v>43910</v>
       </c>
@@ -21062,7 +21187,7 @@
       <c r="N7" s="12"/>
       <c r="O7" s="12"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A8" s="35">
         <v>43911</v>
       </c>
@@ -21085,7 +21210,7 @@
       <c r="N8" s="12"/>
       <c r="O8" s="12"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A9" s="35">
         <v>43912</v>
       </c>
@@ -21108,7 +21233,7 @@
       <c r="N9" s="12"/>
       <c r="O9" s="12"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A10" s="35">
         <v>43913</v>
       </c>
@@ -21131,7 +21256,7 @@
       <c r="N10" s="12"/>
       <c r="O10" s="12"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A11" s="35">
         <v>43914</v>
       </c>
@@ -21154,7 +21279,7 @@
       <c r="N11" s="12"/>
       <c r="O11" s="12"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A12" s="35">
         <v>43915</v>
       </c>
@@ -21177,7 +21302,7 @@
       <c r="N12" s="12"/>
       <c r="O12" s="12"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A13" s="35">
         <v>43916</v>
       </c>
@@ -21200,7 +21325,7 @@
       <c r="N13" s="12"/>
       <c r="O13" s="12"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A14" s="35">
         <v>43917</v>
       </c>
@@ -21223,7 +21348,7 @@
       <c r="N14" s="12"/>
       <c r="O14" s="12"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A15" s="35">
         <v>43918</v>
       </c>
@@ -21246,7 +21371,7 @@
       <c r="N15" s="12"/>
       <c r="O15" s="12"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A16" s="35">
         <v>43919</v>
       </c>
@@ -21269,7 +21394,7 @@
       <c r="N16" s="12"/>
       <c r="O16" s="12"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A17" s="35">
         <v>43920</v>
       </c>
@@ -21292,7 +21417,7 @@
       <c r="N17" s="12"/>
       <c r="O17" s="12"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A18" s="35">
         <v>43921</v>
       </c>
@@ -21315,7 +21440,7 @@
       <c r="N18" s="12"/>
       <c r="O18" s="12"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A19" s="35">
         <v>43922</v>
       </c>
@@ -21338,7 +21463,7 @@
       <c r="N19" s="12"/>
       <c r="O19" s="12"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A20" s="35">
         <v>43923</v>
       </c>
@@ -21361,7 +21486,7 @@
       <c r="N20" s="12"/>
       <c r="O20" s="12"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A21" s="35">
         <v>43924</v>
       </c>
@@ -21384,7 +21509,7 @@
       <c r="N21" s="12"/>
       <c r="O21" s="12"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A22" s="35">
         <v>43925</v>
       </c>
@@ -21407,7 +21532,7 @@
       <c r="N22" s="12"/>
       <c r="O22" s="12"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A23" s="35">
         <v>43926</v>
       </c>
@@ -21430,7 +21555,7 @@
       <c r="N23" s="12"/>
       <c r="O23" s="12"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A24" s="35">
         <v>43927</v>
       </c>
@@ -21453,7 +21578,7 @@
       <c r="N24" s="12"/>
       <c r="O24" s="12"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A25" s="35">
         <v>43928</v>
       </c>
@@ -21476,7 +21601,7 @@
       <c r="N25" s="12"/>
       <c r="O25" s="12"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A26" s="35">
         <v>43929</v>
       </c>
@@ -21499,7 +21624,7 @@
       <c r="N26" s="12"/>
       <c r="O26" s="12"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A27" s="35">
         <v>43930</v>
       </c>
@@ -21691,6 +21816,17 @@
       </c>
       <c r="C40" s="2">
         <v>420</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="36">
+        <v>43944</v>
+      </c>
+      <c r="B41" s="72">
+        <v>3009</v>
+      </c>
+      <c r="C41" s="2">
+        <v>364</v>
       </c>
     </row>
   </sheetData>
@@ -21736,13 +21872,13 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:S41"/>
+  <dimension ref="A1:S42"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F28" sqref="F28"/>
+      <selection pane="bottomRight" activeCell="E42" sqref="E42:F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21751,7 +21887,7 @@
     <col min="2" max="7" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
@@ -21765,7 +21901,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -21810,7 +21946,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A5" s="18">
         <v>43908</v>
       </c>
@@ -21837,7 +21973,7 @@
       <c r="R5" s="12"/>
       <c r="S5" s="12"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A6" s="19">
         <v>43909</v>
       </c>
@@ -21864,7 +22000,7 @@
       <c r="R6" s="12"/>
       <c r="S6" s="12"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A7" s="19">
         <v>43910</v>
       </c>
@@ -21891,7 +22027,7 @@
       <c r="R7" s="12"/>
       <c r="S7" s="12"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A8" s="19">
         <v>43911</v>
       </c>
@@ -21918,7 +22054,7 @@
       <c r="R8" s="12"/>
       <c r="S8" s="12"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A9" s="19">
         <v>43912</v>
       </c>
@@ -21945,7 +22081,7 @@
       <c r="R9" s="12"/>
       <c r="S9" s="12"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A10" s="19">
         <v>43913</v>
       </c>
@@ -21972,7 +22108,7 @@
       <c r="R10" s="12"/>
       <c r="S10" s="12"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A11" s="19">
         <v>43914</v>
       </c>
@@ -21999,7 +22135,7 @@
       <c r="R11" s="12"/>
       <c r="S11" s="12"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A12" s="19">
         <v>43915</v>
       </c>
@@ -22026,7 +22162,7 @@
       <c r="R12" s="12"/>
       <c r="S12" s="12"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A13" s="19">
         <v>43916</v>
       </c>
@@ -22053,7 +22189,7 @@
       <c r="R13" s="12"/>
       <c r="S13" s="12"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A14" s="19">
         <v>43917</v>
       </c>
@@ -22088,7 +22224,7 @@
       <c r="R14" s="12"/>
       <c r="S14" s="12"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A15" s="19">
         <v>43918</v>
       </c>
@@ -22123,7 +22259,7 @@
       <c r="R15" s="12"/>
       <c r="S15" s="12"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A16" s="19">
         <v>43919</v>
       </c>
@@ -22158,7 +22294,7 @@
       <c r="R16" s="12"/>
       <c r="S16" s="12"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A17" s="19">
         <v>43920</v>
       </c>
@@ -22193,7 +22329,7 @@
       <c r="R17" s="12"/>
       <c r="S17" s="12"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A18" s="19">
         <v>43921</v>
       </c>
@@ -22228,7 +22364,7 @@
       <c r="R18" s="12"/>
       <c r="S18" s="12"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A19" s="19">
         <v>43922</v>
       </c>
@@ -22263,7 +22399,7 @@
       <c r="R19" s="12"/>
       <c r="S19" s="12"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A20" s="19">
         <v>43923</v>
       </c>
@@ -22298,7 +22434,7 @@
       <c r="R20" s="12"/>
       <c r="S20" s="12"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A21" s="19">
         <v>43924</v>
       </c>
@@ -22333,7 +22469,7 @@
       <c r="R21" s="12"/>
       <c r="S21" s="12"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A22" s="19">
         <v>43925</v>
       </c>
@@ -22368,7 +22504,7 @@
       <c r="R22" s="12"/>
       <c r="S22" s="12"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A23" s="19">
         <v>43926</v>
       </c>
@@ -22403,7 +22539,7 @@
       <c r="R23" s="12"/>
       <c r="S23" s="12"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A24" s="19">
         <v>43927</v>
       </c>
@@ -22438,7 +22574,7 @@
       <c r="R24" s="12"/>
       <c r="S24" s="12"/>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A25" s="19">
         <v>43928</v>
       </c>
@@ -22473,7 +22609,7 @@
       <c r="R25" s="12"/>
       <c r="S25" s="12"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A26" s="19">
         <v>43929</v>
       </c>
@@ -22508,7 +22644,7 @@
       <c r="R26" s="12"/>
       <c r="S26" s="12"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A27" s="19">
         <v>43930</v>
       </c>
@@ -22543,7 +22679,7 @@
       <c r="R27" s="12"/>
       <c r="S27" s="12"/>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A28" s="19">
         <v>43931</v>
       </c>
@@ -22578,7 +22714,7 @@
       <c r="R28" s="12"/>
       <c r="S28" s="12"/>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A29" s="21">
         <v>43932</v>
       </c>
@@ -22613,7 +22749,7 @@
       <c r="R29" s="12"/>
       <c r="S29" s="12"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A30" s="21">
         <v>43933</v>
       </c>
@@ -22636,7 +22772,7 @@
         <v>1755</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A31" s="57">
         <v>43934</v>
       </c>
@@ -22659,7 +22795,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A32" s="21">
         <v>43935</v>
       </c>
@@ -22682,7 +22818,7 @@
         <v>1801</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A33" s="21">
         <v>43936</v>
       </c>
@@ -22705,7 +22841,7 @@
         <v>1747</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A34" s="80">
         <v>43937</v>
       </c>
@@ -22867,26 +23003,49 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="84">
+      <c r="A41" s="82">
         <v>43944</v>
       </c>
-      <c r="B41" s="103">
+      <c r="B41" s="105">
         <v>136</v>
       </c>
-      <c r="C41" s="103">
+      <c r="C41" s="105">
         <v>12</v>
       </c>
-      <c r="D41" s="104">
+      <c r="D41" s="98">
         <v>148</v>
       </c>
-      <c r="E41" s="136">
+      <c r="E41" s="99">
         <v>1423</v>
       </c>
-      <c r="F41" s="104">
+      <c r="F41" s="98">
         <v>325</v>
       </c>
-      <c r="G41" s="104">
+      <c r="G41" s="98">
         <v>1748</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="84">
+        <v>43945</v>
+      </c>
+      <c r="B42" s="103">
+        <v>136</v>
+      </c>
+      <c r="C42" s="103">
+        <v>5</v>
+      </c>
+      <c r="D42" s="104">
+        <v>141</v>
+      </c>
+      <c r="E42" s="136">
+        <v>1383</v>
+      </c>
+      <c r="F42" s="104">
+        <v>327</v>
+      </c>
+      <c r="G42" s="104">
+        <v>1710</v>
       </c>
     </row>
   </sheetData>
@@ -22909,9 +23068,9 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:AC38"/>
+  <dimension ref="A1:AC39"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="G3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="F3" sqref="A1:F1048576"/>
     </sheetView>
   </sheetViews>
@@ -22925,7 +23084,7 @@
     <col min="6" max="6" width="8.85546875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="60" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" s="60" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
@@ -22958,7 +23117,7 @@
       <c r="AB1" s="61"/>
       <c r="AC1" s="61"/>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A2" s="62">
         <v>43908</v>
       </c>
@@ -22993,7 +23152,7 @@
       <c r="AB2" s="65"/>
       <c r="AC2" s="65"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A3" s="62">
         <f>A2+1</f>
         <v>43909</v>
@@ -23029,7 +23188,7 @@
       <c r="AB3" s="65"/>
       <c r="AC3" s="65"/>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A4" s="62">
         <f t="shared" ref="A4:A20" si="0">A3+1</f>
         <v>43910</v>
@@ -23065,7 +23224,7 @@
       <c r="AB4" s="65"/>
       <c r="AC4" s="65"/>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A5" s="62">
         <f t="shared" si="0"/>
         <v>43911</v>
@@ -23101,7 +23260,7 @@
       <c r="AB5" s="65"/>
       <c r="AC5" s="65"/>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A6" s="62">
         <f t="shared" si="0"/>
         <v>43912</v>
@@ -23136,7 +23295,7 @@
       <c r="AB6" s="65"/>
       <c r="AC6" s="65"/>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A7" s="62">
         <f t="shared" si="0"/>
         <v>43913</v>
@@ -23157,7 +23316,7 @@
       </c>
       <c r="F7" s="66"/>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A8" s="62">
         <f t="shared" si="0"/>
         <v>43914</v>
@@ -23178,7 +23337,7 @@
       </c>
       <c r="F8" s="66"/>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A9" s="62">
         <f t="shared" si="0"/>
         <v>43915</v>
@@ -23199,7 +23358,7 @@
       </c>
       <c r="F9" s="66"/>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A10" s="62">
         <f t="shared" si="0"/>
         <v>43916</v>
@@ -23218,7 +23377,7 @@
       </c>
       <c r="F10" s="66"/>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A11" s="62">
         <f t="shared" si="0"/>
         <v>43917</v>
@@ -23236,7 +23395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A12" s="62">
         <f t="shared" si="0"/>
         <v>43918</v>
@@ -23254,7 +23413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A13" s="62">
         <f t="shared" si="0"/>
         <v>43919</v>
@@ -23272,7 +23431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A14" s="62">
         <f t="shared" si="0"/>
         <v>43920</v>
@@ -23290,7 +23449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A15" s="62">
         <f t="shared" si="0"/>
         <v>43921</v>
@@ -23308,7 +23467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A16" s="62">
         <f t="shared" si="0"/>
         <v>43922</v>
@@ -23326,7 +23485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A17" s="62">
         <f t="shared" si="0"/>
         <v>43923</v>
@@ -23344,7 +23503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A18" s="62">
         <f t="shared" si="0"/>
         <v>43924</v>
@@ -23362,7 +23521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A19" s="62">
         <f t="shared" si="0"/>
         <v>43925</v>
@@ -23380,7 +23539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A20" s="62">
         <f t="shared" si="0"/>
         <v>43926</v>
@@ -23398,7 +23557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A21" s="62">
         <v>43927</v>
       </c>
@@ -23760,6 +23919,23 @@
         <v>325</v>
       </c>
       <c r="E38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A39" s="62">
+        <v>43945</v>
+      </c>
+      <c r="B39">
+        <v>1710</v>
+      </c>
+      <c r="C39">
+        <v>1383</v>
+      </c>
+      <c r="D39">
+        <v>327</v>
+      </c>
+      <c r="E39">
         <v>0</v>
       </c>
     </row>
@@ -23781,8 +23957,8 @@
   </sheetPr>
   <dimension ref="A1:AD82"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F29" sqref="A1:F1048576"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="P41" sqref="P41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23796,7 +23972,7 @@
     <col min="10" max="10" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="60" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" s="60" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
@@ -23830,7 +24006,7 @@
       <c r="AC1" s="61"/>
       <c r="AD1" s="61"/>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A2" s="62">
         <v>43908</v>
       </c>
@@ -23866,7 +24042,7 @@
       <c r="AC2" s="65"/>
       <c r="AD2" s="65"/>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A3" s="62">
         <f>A2+1</f>
         <v>43909</v>
@@ -23903,7 +24079,7 @@
       <c r="AC3" s="65"/>
       <c r="AD3" s="65"/>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A4" s="62">
         <f t="shared" ref="A4:A20" si="0">A3+1</f>
         <v>43910</v>
@@ -23940,7 +24116,7 @@
       <c r="AC4" s="65"/>
       <c r="AD4" s="65"/>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A5" s="62">
         <f t="shared" si="0"/>
         <v>43911</v>
@@ -23977,7 +24153,7 @@
       <c r="AC5" s="65"/>
       <c r="AD5" s="65"/>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A6" s="62">
         <f t="shared" si="0"/>
         <v>43912</v>
@@ -24013,7 +24189,7 @@
       <c r="AC6" s="65"/>
       <c r="AD6" s="65"/>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A7" s="62">
         <f t="shared" si="0"/>
         <v>43913</v>
@@ -24049,7 +24225,7 @@
       <c r="AC7" s="65"/>
       <c r="AD7" s="65"/>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A8" s="62">
         <f t="shared" si="0"/>
         <v>43914</v>
@@ -24070,7 +24246,7 @@
       </c>
       <c r="F8" s="70"/>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A9" s="62">
         <f t="shared" si="0"/>
         <v>43915</v>
@@ -24091,7 +24267,7 @@
       </c>
       <c r="F9" s="66"/>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A10" s="62">
         <f t="shared" si="0"/>
         <v>43916</v>
@@ -24110,7 +24286,7 @@
       </c>
       <c r="F10" s="66"/>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A11" s="62">
         <f t="shared" si="0"/>
         <v>43917</v>
@@ -24128,7 +24304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A12" s="62">
         <f t="shared" si="0"/>
         <v>43918</v>
@@ -24146,7 +24322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A13" s="62">
         <f t="shared" si="0"/>
         <v>43919</v>
@@ -24164,7 +24340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A14" s="62">
         <f t="shared" si="0"/>
         <v>43920</v>
@@ -24182,7 +24358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A15" s="62">
         <f t="shared" si="0"/>
         <v>43921</v>
@@ -24200,7 +24376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A16" s="62">
         <f t="shared" si="0"/>
         <v>43922</v>
@@ -24218,7 +24394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A17" s="62">
         <f t="shared" si="0"/>
         <v>43923</v>
@@ -24236,7 +24412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A18" s="62">
         <f t="shared" si="0"/>
         <v>43924</v>
@@ -24254,7 +24430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A19" s="62">
         <f t="shared" si="0"/>
         <v>43925</v>
@@ -24272,7 +24448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A20" s="62">
         <f t="shared" si="0"/>
         <v>43926</v>
@@ -24290,7 +24466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A21" s="62">
         <v>43927</v>
       </c>
@@ -24663,6 +24839,23 @@
         <v>12</v>
       </c>
       <c r="E38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A39" s="62">
+        <v>43945</v>
+      </c>
+      <c r="B39">
+        <v>141</v>
+      </c>
+      <c r="C39">
+        <v>136</v>
+      </c>
+      <c r="D39">
+        <v>5</v>
+      </c>
+      <c r="E39">
         <v>0</v>
       </c>
     </row>
@@ -24748,10 +24941,10 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:P39"/>
+  <dimension ref="A1:P44"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight"/>
@@ -24765,7 +24958,7 @@
     <col min="4" max="4" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>40</v>
       </c>
@@ -24776,13 +24969,13 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:16" ht="39" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="40.700000000000003" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>0</v>
       </c>
@@ -24797,7 +24990,7 @@
       </c>
       <c r="E3" s="45"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A4" s="18">
         <v>43908</v>
       </c>
@@ -24823,7 +25016,7 @@
       <c r="O4" s="12"/>
       <c r="P4" s="12"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A5" s="19">
         <v>43909</v>
       </c>
@@ -24849,7 +25042,7 @@
       <c r="O5" s="12"/>
       <c r="P5" s="12"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A6" s="19">
         <v>43910</v>
       </c>
@@ -24875,7 +25068,7 @@
       <c r="O6" s="12"/>
       <c r="P6" s="12"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A7" s="19">
         <v>43911</v>
       </c>
@@ -24901,7 +25094,7 @@
       <c r="O7" s="12"/>
       <c r="P7" s="12"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A8" s="19">
         <v>43912</v>
       </c>
@@ -24927,7 +25120,7 @@
       <c r="O8" s="12"/>
       <c r="P8" s="12"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A9" s="19">
         <v>43913</v>
       </c>
@@ -24953,7 +25146,7 @@
       <c r="O9" s="12"/>
       <c r="P9" s="12"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A10" s="19">
         <v>43914</v>
       </c>
@@ -24979,7 +25172,7 @@
       <c r="O10" s="12"/>
       <c r="P10" s="12"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A11" s="19">
         <v>43915</v>
       </c>
@@ -25005,7 +25198,7 @@
       <c r="O11" s="12"/>
       <c r="P11" s="12"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A12" s="19">
         <v>43916</v>
       </c>
@@ -25031,7 +25224,7 @@
       <c r="O12" s="12"/>
       <c r="P12" s="12"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A13" s="19">
         <v>43917</v>
       </c>
@@ -25057,7 +25250,7 @@
       <c r="O13" s="12"/>
       <c r="P13" s="12"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A14" s="19">
         <v>43918</v>
       </c>
@@ -25083,7 +25276,7 @@
       <c r="O14" s="12"/>
       <c r="P14" s="12"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A15" s="19">
         <v>43919</v>
       </c>
@@ -25109,7 +25302,7 @@
       <c r="O15" s="12"/>
       <c r="P15" s="12"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A16" s="19">
         <v>43920</v>
       </c>
@@ -25135,7 +25328,7 @@
       <c r="O16" s="12"/>
       <c r="P16" s="12"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A17" s="19">
         <v>43921</v>
       </c>
@@ -25161,7 +25354,7 @@
       <c r="O17" s="12"/>
       <c r="P17" s="12"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A18" s="19">
         <v>43922</v>
       </c>
@@ -25187,7 +25380,7 @@
       <c r="O18" s="12"/>
       <c r="P18" s="12"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A19" s="19">
         <v>43923</v>
       </c>
@@ -25213,7 +25406,7 @@
       <c r="O19" s="12"/>
       <c r="P19" s="12"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A20" s="19">
         <v>43924</v>
       </c>
@@ -25239,7 +25432,7 @@
       <c r="O20" s="12"/>
       <c r="P20" s="12"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A21" s="19">
         <v>43925</v>
       </c>
@@ -25265,7 +25458,7 @@
       <c r="O21" s="12"/>
       <c r="P21" s="12"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A22" s="19">
         <v>43926</v>
       </c>
@@ -25291,7 +25484,7 @@
       <c r="O22" s="12"/>
       <c r="P22" s="12"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A23" s="19">
         <v>43927</v>
       </c>
@@ -25317,7 +25510,7 @@
       <c r="O23" s="12"/>
       <c r="P23" s="12"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A24" s="19">
         <v>43928</v>
       </c>
@@ -25343,7 +25536,7 @@
       <c r="O24" s="12"/>
       <c r="P24" s="12"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A25" s="19">
         <v>43929</v>
       </c>
@@ -25369,7 +25562,7 @@
       <c r="O25" s="12"/>
       <c r="P25" s="12"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A26" s="19">
         <v>43930</v>
       </c>
@@ -25395,7 +25588,7 @@
       <c r="O26" s="12"/>
       <c r="P26" s="12"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A27" s="19">
         <v>43931</v>
       </c>
@@ -25421,7 +25614,7 @@
       <c r="O27" s="12"/>
       <c r="P27" s="12"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A28" s="21">
         <v>43932</v>
       </c>
@@ -25447,7 +25640,7 @@
       <c r="O28" s="12"/>
       <c r="P28" s="12"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A29" s="21">
         <v>43933</v>
       </c>
@@ -25462,7 +25655,7 @@
       </c>
       <c r="E29" s="45"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A30" s="21">
         <v>43934</v>
       </c>
@@ -25604,6 +25797,44 @@
       <c r="D39" s="9">
         <v>192</v>
       </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="21">
+        <v>43944</v>
+      </c>
+      <c r="B40" s="72">
+        <v>1489</v>
+      </c>
+      <c r="C40" s="72">
+        <v>327</v>
+      </c>
+      <c r="D40" s="81">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -25629,7 +25860,7 @@
     <col min="1" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A1" s="46"/>
       <c r="P1" s="33" t="s">
         <v>35</v>
@@ -25645,7 +25876,7 @@
 </worksheet>
 </file>
 
-<file path=customXML/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXML/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://www.objective.com/ecm/document/metadata/53D26341A57B383EE0540010E0463CCA" version="1.0.0">
   <systemFields>
     <field name="Objective-Id">
@@ -25667,10 +25898,10 @@
       <value order="0">true</value>
     </field>
     <field name="Objective-DatePublished">
-      <value order="0">2020-04-23T12:03:19Z</value>
+      <value order="0">2020-04-24T12:50:44Z</value>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2020-04-23T12:03:20Z</value>
+      <value order="0">2020-04-24T12:50:44Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Munro, Fraser F (Z615428)</value>
@@ -25685,13 +25916,13 @@
       <value order="0">Published</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA40720023</value>
+      <value order="0">vA40749732</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">9.0</value>
+      <value order="0">10.0</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">114</value>
+      <value order="0">125</value>
     </field>
     <field name="Objective-VersionComment">
       <value order="0"/>
@@ -25728,7 +25959,7 @@
 </metadata>
 </file>
 
-<file path=customXML/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXML/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5745109E-2DDF-40CB-AC2B-FF9B10C90820}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.objective.com/ecm/document/metadata/53D26341A57B383EE0540010E0463CCA"/>

</xml_diff>